<commit_message>
polished, make all deliverables
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -46,10 +46,10 @@
     <t>&lt;Parameter prj not found&gt;</t>
   </si>
   <si>
-    <t>17/10/2015</t>
-  </si>
-  <si>
-    <t>14:07:50</t>
+    <t>19/10/2015</t>
+  </si>
+  <si>
+    <t>10:42:12</t>
   </si>
   <si>
     <t>&lt;Parameter OrderQty not found&gt;</t>
@@ -1576,7 +1576,7 @@
         <v>165</v>
       </c>
       <c r="L5" s="12">
-        <v>4227218</v>
+        <v>4226408</v>
       </c>
       <c r="M5" s="33" t="s">
         <v>171</v>
@@ -1832,7 +1832,7 @@
         <v>165</v>
       </c>
       <c r="L9" s="12">
-        <v>197148</v>
+        <v>197098</v>
       </c>
       <c r="M9" s="33" t="s">
         <v>174</v>
@@ -2024,7 +2024,7 @@
         <v>165</v>
       </c>
       <c r="L12" s="12">
-        <v>8958</v>
+        <v>8920</v>
       </c>
       <c r="M12" s="33" t="s">
         <v>176</v>
@@ -2088,7 +2088,7 @@
         <v>165</v>
       </c>
       <c r="L13" s="12">
-        <v>10068</v>
+        <v>9321</v>
       </c>
       <c r="M13" s="33" t="s">
         <v>177</v>
@@ -2152,7 +2152,7 @@
         <v>165</v>
       </c>
       <c r="L14" s="12">
-        <v>13467</v>
+        <v>13567</v>
       </c>
       <c r="M14" s="33" t="s">
         <v>178</v>
@@ -2344,7 +2344,7 @@
         <v>165</v>
       </c>
       <c r="L17" s="12">
-        <v>1575557</v>
+        <v>1575457</v>
       </c>
       <c r="M17" s="33" t="s">
         <v>180</v>
@@ -2408,7 +2408,7 @@
         <v>165</v>
       </c>
       <c r="L18" s="12">
-        <v>48885</v>
+        <v>48690</v>
       </c>
       <c r="M18" s="33" t="s">
         <v>181</v>
@@ -2472,7 +2472,7 @@
         <v>165</v>
       </c>
       <c r="L19" s="12">
-        <v>61788</v>
+        <v>61778</v>
       </c>
       <c r="M19" s="33" t="s">
         <v>182</v>
@@ -2536,7 +2536,7 @@
         <v>165</v>
       </c>
       <c r="L20" s="12">
-        <v>1844591</v>
+        <v>1844557</v>
       </c>
       <c r="M20" s="33" t="s">
         <v>183</v>
@@ -2664,7 +2664,7 @@
         <v>165</v>
       </c>
       <c r="L22" s="12">
-        <v>1232611</v>
+        <v>1232071</v>
       </c>
       <c r="M22" s="33" t="s">
         <v>185</v>
@@ -3292,7 +3292,7 @@
       <c r="L33" s="17"/>
       <c r="M33" s="39">
         <f ca="1">NOW()</f>
-        <v>42294.588871990738</v>
+        <v>42296.446042824071</v>
       </c>
       <c r="N33" s="45"/>
       <c r="O33" s="18"/>

</xml_diff>

<commit_message>
all supplier info for parts previously 0402 removed [to update for 0603]
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="168">
   <si>
     <t>Item #</t>
   </si>
@@ -43,16 +43,19 @@
     <t>Adjusted Supplier Subtotal 1</t>
   </si>
   <si>
-    <t>&lt;Parameter prj not found&gt;</t>
+    <t>per board</t>
+  </si>
+  <si>
+    <t>n-baseU68</t>
   </si>
   <si>
     <t>19/10/2015</t>
   </si>
   <si>
-    <t>10:42:12</t>
-  </si>
-  <si>
-    <t>&lt;Parameter OrderQty not found&gt;</t>
+    <t>11:25:59</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
   <si>
     <t>Designator</t>
@@ -64,34 +67,64 @@
     <t>C11</t>
   </si>
   <si>
+    <t>C2, C3, C4, C5, C12</t>
+  </si>
+  <si>
+    <t>C7, C9</t>
+  </si>
+  <si>
+    <t>C8, C10</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2, D3, D4, D5, D6, D7</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>R3, R4, R8, R13</t>
+  </si>
+  <si>
+    <t>R9, R10</t>
+  </si>
+  <si>
+    <t>SW1, SW2, SW3</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
     <t>C14</t>
   </si>
   <si>
     <t>C15</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C12</t>
-  </si>
-  <si>
     <t>C6</t>
   </si>
   <si>
-    <t>C7, C9</t>
-  </si>
-  <si>
-    <t>C8, C10</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2, D3, D4, D5, D6, D7</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>JP2</t>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>JP4</t>
   </si>
   <si>
     <t>LD1</t>
@@ -112,39 +145,9 @@
     <t>R12, R14</t>
   </si>
   <si>
-    <t>R3, R4, R8, R13</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
-    <t>R9, R10</t>
-  </si>
-  <si>
-    <t>SW1, SW2, SW3</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>JP4</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -157,28 +160,58 @@
     <t>0.011F</t>
   </si>
   <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>7pF</t>
+  </si>
+  <si>
+    <t>1uF/MLCC</t>
+  </si>
+  <si>
+    <t>NSR20F30NXT5G</t>
+  </si>
+  <si>
+    <t>USB-MINI-B</t>
+  </si>
+  <si>
+    <t>Header 5X2 1.27mm</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>EVQ-P2202M</t>
+  </si>
+  <si>
+    <t>TPS78233</t>
+  </si>
+  <si>
+    <t>FC135-32.76KAA3</t>
+  </si>
+  <si>
+    <t>LPC11U68JBD48</t>
+  </si>
+  <si>
+    <t>12MHz/10pF</t>
+  </si>
+  <si>
+    <t>N-GMS</t>
+  </si>
+  <si>
     <t>10uF/MLCC</t>
   </si>
   <si>
-    <t>100nF</t>
-  </si>
-  <si>
     <t>18pF</t>
   </si>
   <si>
-    <t>7pF</t>
-  </si>
-  <si>
-    <t>1uF/MLCC</t>
-  </si>
-  <si>
-    <t>NSR20F30NXT5G</t>
-  </si>
-  <si>
-    <t>USB-MINI-B</t>
-  </si>
-  <si>
-    <t>Header 5X2 1.27mm</t>
+    <t>HEADER-2</t>
+  </si>
+  <si>
+    <t>HEADER_5</t>
   </si>
   <si>
     <t>LED_RED</t>
@@ -190,9 +223,6 @@
     <t>LED_BLU</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>620R</t>
   </si>
   <si>
@@ -202,33 +232,6 @@
     <t>18K</t>
   </si>
   <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>EVQ-P2202M</t>
-  </si>
-  <si>
-    <t>TPS78233</t>
-  </si>
-  <si>
-    <t>FC135-32.76KAA3</t>
-  </si>
-  <si>
-    <t>LPC11U68JBD48</t>
-  </si>
-  <si>
-    <t>12MHz/10pF</t>
-  </si>
-  <si>
-    <t>N-GMS</t>
-  </si>
-  <si>
-    <t>HEADER-2</t>
-  </si>
-  <si>
-    <t>HEADER_5</t>
-  </si>
-  <si>
     <t>N-NODE24-20pin</t>
   </si>
   <si>
@@ -256,6 +259,30 @@
     <t>2x5-1.27mm-HARWIN-855-M50-3600542</t>
   </si>
   <si>
+    <t>0603_res</t>
+  </si>
+  <si>
+    <t>BUTTON_4.7x3.5mm</t>
+  </si>
+  <si>
+    <t>SOT23-5_0.95mm-NOSILK</t>
+  </si>
+  <si>
+    <t>CRYSTAL-3.2x1.5</t>
+  </si>
+  <si>
+    <t>SOT313-2_V</t>
+  </si>
+  <si>
+    <t>CRY-SMD4-EPSON-FA238V</t>
+  </si>
+  <si>
+    <t>1X02</t>
+  </si>
+  <si>
+    <t>1X05</t>
+  </si>
+  <si>
     <t>0603_LED_RED</t>
   </si>
   <si>
@@ -265,30 +292,6 @@
     <t>0603_LED_BLU</t>
   </si>
   <si>
-    <t>0603_res</t>
-  </si>
-  <si>
-    <t>BUTTON_4.7x3.5mm</t>
-  </si>
-  <si>
-    <t>SOT23-5_0.95mm-NOSILK</t>
-  </si>
-  <si>
-    <t>CRYSTAL-3.2x1.5</t>
-  </si>
-  <si>
-    <t>SOT313-2_V</t>
-  </si>
-  <si>
-    <t>CRY-SMD4-EPSON-FA238V</t>
-  </si>
-  <si>
-    <t>1X02</t>
-  </si>
-  <si>
-    <t>1X05</t>
-  </si>
-  <si>
     <t>N-NODE24-20pins</t>
   </si>
   <si>
@@ -328,18 +331,9 @@
     <t>Supercapacitors / Ultracapacitors SUPER CAP 3.3V 0.011F</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 10UF 6.3V 20% 0402</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 0.1uF 16volts X7R 10%</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 0.1uF 10% X7R</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0402 18pF 25volts C0G 5%</t>
-  </si>
-  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 1.0uF 16volts X7R 10%</t>
   </si>
   <si>
@@ -352,27 +346,9 @@
     <t>Headers &amp; Wire Housings 5+5 DIL PIN HDR SMT Au/Sn</t>
   </si>
   <si>
-    <t>Standard LEDs - SMD 0402 SUPER RED Non-Diff</t>
-  </si>
-  <si>
-    <t>Standard LEDs - SMD 0402 GREEN Non-Diff</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 1/16watt 10Kohms 1%</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 1/16watt 680ohms 1%</t>
-  </si>
-  <si>
-    <t>Thick Film Resistors - SMD 1/16watt 470ohms 1% 100ppm</t>
-  </si>
-  <si>
     <t>Thick Film Resistors - SMD 0603 10Kohms 1% Tol</t>
   </si>
   <si>
-    <t>Thick Film Resistors - SMD 1/16watt 18.2Kohms 1%</t>
-  </si>
-  <si>
     <t>Thick Film Resistors - SMD 0603 Zero Ohms</t>
   </si>
   <si>
@@ -412,12 +388,6 @@
     <t>Harwin</t>
   </si>
   <si>
-    <t>Vishay Semiconductors</t>
-  </si>
-  <si>
-    <t>Vishay / Dale</t>
-  </si>
-  <si>
     <t>Panasonic</t>
   </si>
   <si>
@@ -442,18 +412,9 @@
     <t>PAS3225P3R3113</t>
   </si>
   <si>
-    <t>GRM155R60J106ME44D</t>
-  </si>
-  <si>
-    <t>GRM155R71C104KA88D</t>
-  </si>
-  <si>
     <t>06035C104KAT2A</t>
   </si>
   <si>
-    <t>GRM1555C1E180JA01D</t>
-  </si>
-  <si>
     <t>GCM188R71C105KA64D</t>
   </si>
   <si>
@@ -463,27 +424,9 @@
     <t>M50-3600542</t>
   </si>
   <si>
-    <t>VLMS1500-GS08</t>
-  </si>
-  <si>
-    <t>VLMG1500-GS08</t>
-  </si>
-  <si>
-    <t>CRCW040210K0FKED</t>
-  </si>
-  <si>
-    <t>CRCW0402680RFKED</t>
-  </si>
-  <si>
-    <t>CRCW0402470RFKED</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
-    <t>CRCW040218K2FKED</t>
-  </si>
-  <si>
     <t>ERJ-3GEY0R00V</t>
   </si>
   <si>
@@ -526,18 +469,9 @@
     <t>963-PAS3225P3R3113</t>
   </si>
   <si>
-    <t>81-GRM155R60J106ME4D</t>
-  </si>
-  <si>
-    <t>81-GRM155R71C104KA88</t>
-  </si>
-  <si>
     <t>581-06035C104KAT2A</t>
   </si>
   <si>
-    <t>81-GRM1555C1E180JA1D</t>
-  </si>
-  <si>
     <t>81-GCM188R71C105K64D</t>
   </si>
   <si>
@@ -550,25 +484,7 @@
     <t>855-M50-3600542</t>
   </si>
   <si>
-    <t>78-VLMS1500-GS08</t>
-  </si>
-  <si>
-    <t>78-VLMG1500-GS08</t>
-  </si>
-  <si>
-    <t>71-CRCW0402-10K-E3</t>
-  </si>
-  <si>
-    <t>71-CRCW0402-680-E3</t>
-  </si>
-  <si>
-    <t>71-CRCW0402-470-E3</t>
-  </si>
-  <si>
     <t>667-ERJ-3EKF1002V</t>
-  </si>
-  <si>
-    <t>71-CRCW0402-18.2K-E3</t>
   </si>
   <si>
     <t>667-ERJ-3GEY0R00V</t>
@@ -733,7 +649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -815,11 +731,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -947,6 +889,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1264,7 +1210,7 @@
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T4"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1286,6 +1232,7 @@
     <col min="16" max="17" width="6.42578125" style="32" customWidth="1"/>
     <col min="18" max="18" width="10.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1293,55 +1240,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>194</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>8</v>
@@ -1356,41 +1303,41 @@
         <v>1</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L2" s="12">
-        <v>210127</v>
+        <v>210123</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="N2" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O2" s="12">
         <v>1</v>
@@ -1420,41 +1367,41 @@
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L3" s="12">
         <v>6237</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="N3" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O3" s="12">
         <v>1</v>
@@ -1484,58 +1431,58 @@
         <v>3</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L4" s="12">
-        <v>190926</v>
+        <v>483363</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="N4" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O4" s="12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P4" s="13">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="Q4" s="13">
         <f>ROUNDUP(P4*N4,0)</f>
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="R4" s="34">
-        <v>0.20399999999999999</v>
+        <v>2.7E-2</v>
       </c>
       <c r="S4" s="34">
         <f>R4*Q4</f>
-        <v>5.0999999999999996</v>
+        <v>3.375</v>
       </c>
       <c r="T4" s="9">
         <f>ROW(T4) - ROW($A$1)</f>
@@ -1548,58 +1495,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>162</v>
-      </c>
       <c r="K5" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L5" s="12">
-        <v>4226408</v>
+        <v>210123</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="N5" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O5" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P5" s="13">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q5" s="13">
         <f t="shared" ref="Q5" si="4">ROUNDUP(P5*N5,0)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="R5" s="34">
-        <v>1.2999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="S5" s="34">
         <f t="shared" ref="S5" si="5">R5*Q5</f>
-        <v>0.32500000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" si="3"/>
@@ -1612,58 +1559,58 @@
         <v>5</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G6" s="38" t="s">
         <v>106</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L6" s="12">
-        <v>483363</v>
+        <v>197098</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="N6" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O6" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P6" s="13">
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="Q6" s="13">
         <f>ROUNDUP(P6*N6,0)</f>
-        <v>125</v>
+        <v>50</v>
       </c>
       <c r="R6" s="34">
-        <v>2.7E-2</v>
+        <v>0.151</v>
       </c>
       <c r="S6" s="34">
         <f>R6*Q6</f>
-        <v>3.375</v>
+        <v>7.55</v>
       </c>
       <c r="T6" s="9">
         <f>ROW(T6) - ROW($A$1)</f>
@@ -1676,41 +1623,41 @@
         <v>6</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G7" s="38" t="s">
         <v>107</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L7" s="12">
-        <v>65669</v>
+        <v>32441</v>
       </c>
       <c r="M7" s="33" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="N7" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O7" s="12">
         <v>1</v>
@@ -1723,11 +1670,11 @@
         <v>25</v>
       </c>
       <c r="R7" s="34">
-        <v>2.5000000000000001E-2</v>
+        <v>0.33500000000000002</v>
       </c>
       <c r="S7" s="34">
         <f t="shared" ref="S7" si="7">R7*Q7</f>
-        <v>0.625</v>
+        <v>8.375</v>
       </c>
       <c r="T7" s="9">
         <f t="shared" si="3"/>
@@ -1740,58 +1687,58 @@
         <v>7</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>140</v>
+        <v>51</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L8" s="12">
-        <v>210127</v>
+        <v>32441</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="N8" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O8" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P8" s="13">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="Q8" s="13">
         <f>ROUNDUP(P8*N8,0)</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="R8" s="34">
-        <v>0.03</v>
+        <v>0.186</v>
       </c>
       <c r="S8" s="34">
         <f>R8*Q8</f>
-        <v>1.5</v>
+        <v>27.9</v>
       </c>
       <c r="T8" s="9">
         <f>ROW(T8) - ROW($A$1)</f>
@@ -1804,58 +1751,58 @@
         <v>8</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G9" s="38" t="s">
         <v>108</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I9" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>165</v>
-      </c>
       <c r="L9" s="12">
-        <v>197098</v>
+        <v>8920</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="N9" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O9" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P9" s="13">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="13">
         <f t="shared" ref="Q9" si="8">ROUNDUP(P9*N9,0)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="R9" s="34">
-        <v>0.151</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="S9" s="34">
         <f t="shared" ref="S9" si="9">R9*Q9</f>
-        <v>7.55</v>
+        <v>17.175000000000001</v>
       </c>
       <c r="T9" s="9">
         <f t="shared" si="3"/>
@@ -1868,41 +1815,41 @@
         <v>9</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G10" s="38" t="s">
         <v>109</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L10" s="12">
-        <v>32441</v>
+        <v>9321</v>
       </c>
       <c r="M10" s="33" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="N10" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O10" s="12">
         <v>1</v>
@@ -1915,11 +1862,11 @@
         <v>25</v>
       </c>
       <c r="R10" s="34">
-        <v>0.33500000000000002</v>
+        <v>0.874</v>
       </c>
       <c r="S10" s="34">
         <f>R10*Q10</f>
-        <v>8.375</v>
+        <v>21.85</v>
       </c>
       <c r="T10" s="9">
         <f>ROW(T10) - ROW($A$1)</f>
@@ -1932,58 +1879,58 @@
         <v>10</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>52</v>
+        <v>136</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L11" s="12">
-        <v>32441</v>
+        <v>1844557</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="N11" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O11" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P11" s="13">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="13">
         <f t="shared" ref="Q11" si="10">ROUNDUP(P11*N11,0)</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="R11" s="34">
-        <v>0.186</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="S11" s="34">
         <f t="shared" ref="S11" si="11">R11*Q11</f>
-        <v>27.9</v>
+        <v>0.8</v>
       </c>
       <c r="T11" s="9">
         <f t="shared" si="3"/>
@@ -1996,58 +1943,58 @@
         <v>11</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L12" s="12">
-        <v>8920</v>
+        <v>1232071</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="N12" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O12" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12" s="13">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q12" s="13">
         <f>ROUNDUP(P12*N12,0)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="R12" s="34">
-        <v>0.68700000000000006</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="S12" s="34">
         <f>R12*Q12</f>
-        <v>17.175000000000001</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="T12" s="9">
         <f>ROW(T12) - ROW($A$1)</f>
@@ -2060,58 +2007,58 @@
         <v>12</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L13" s="12">
-        <v>9321</v>
+        <v>3171</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="N13" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O13" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P13" s="13">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" ref="Q13" si="12">ROUNDUP(P13*N13,0)</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="R13" s="34">
-        <v>0.874</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="S13" s="34">
         <f t="shared" ref="S13" si="13">R13*Q13</f>
-        <v>21.85</v>
+        <v>44.174999999999997</v>
       </c>
       <c r="T13" s="9">
         <f t="shared" si="3"/>
@@ -2124,41 +2071,41 @@
         <v>13</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L14" s="12">
-        <v>13567</v>
+        <v>12597</v>
       </c>
       <c r="M14" s="33" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="N14" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O14" s="12">
         <v>1</v>
@@ -2171,11 +2118,11 @@
         <v>25</v>
       </c>
       <c r="R14" s="34">
-        <v>0.27800000000000002</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="S14" s="34">
         <f>R14*Q14</f>
-        <v>6.9500000000000011</v>
+        <v>15.950000000000001</v>
       </c>
       <c r="T14" s="9">
         <f>ROW(T14) - ROW($A$1)</f>
@@ -2188,41 +2135,41 @@
         <v>14</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L15" s="12">
-        <v>54548</v>
+        <v>3650</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="N15" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O15" s="12">
         <v>1</v>
@@ -2235,11 +2182,11 @@
         <v>25</v>
       </c>
       <c r="R15" s="34">
-        <v>0.27800000000000002</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="S15" s="34">
         <f t="shared" ref="S15" si="15">R15*Q15</f>
-        <v>6.9500000000000011</v>
+        <v>20.574999999999999</v>
       </c>
       <c r="T15" s="9">
         <f t="shared" si="3"/>
@@ -2252,41 +2199,41 @@
         <v>15</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="L16" s="12">
-        <v>54548</v>
+        <v>-4</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="N16" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O16" s="12">
         <v>1</v>
@@ -2299,11 +2246,11 @@
         <v>25</v>
       </c>
       <c r="R16" s="34">
-        <v>0.27800000000000002</v>
+        <v>4.92</v>
       </c>
       <c r="S16" s="34">
         <f>R16*Q16</f>
-        <v>6.9500000000000011</v>
+        <v>123</v>
       </c>
       <c r="T16" s="9">
         <f>ROW(T16) - ROW($A$1)</f>
@@ -2316,58 +2263,58 @@
         <v>16</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="J17" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="12">
+        <v>7840</v>
+      </c>
+      <c r="M17" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="K17" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L17" s="12">
-        <v>1575457</v>
-      </c>
-      <c r="M17" s="33" t="s">
-        <v>180</v>
-      </c>
       <c r="N17" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O17" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P17" s="13">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" ref="Q17" si="16">ROUNDUP(P17*N17,0)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="R17" s="34">
-        <v>2.4E-2</v>
+        <v>1.34</v>
       </c>
       <c r="S17" s="34">
         <f t="shared" ref="S17" si="17">R17*Q17</f>
-        <v>2.4</v>
+        <v>33.5</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="3"/>
@@ -2380,58 +2327,52 @@
         <v>17</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L18" s="12">
-        <v>48690</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L18" s="12"/>
       <c r="M18" s="33" t="s">
-        <v>181</v>
+        <v>96</v>
       </c>
       <c r="N18" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O18" s="12">
         <v>1</v>
       </c>
-      <c r="P18" s="13">
-        <v>25</v>
-      </c>
+      <c r="P18" s="13"/>
       <c r="Q18" s="13">
         <f>ROUNDUP(P18*N18,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R18" s="34">
-        <v>4.1000000000000002E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R18" s="34"/>
       <c r="S18" s="34">
         <f>R18*Q18</f>
-        <v>1.0250000000000001</v>
+        <v>0</v>
       </c>
       <c r="T18" s="9">
         <f>ROW(T18) - ROW($A$1)</f>
@@ -2444,58 +2385,52 @@
         <v>18</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L19" s="12">
-        <v>61778</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L19" s="12"/>
       <c r="M19" s="33" t="s">
-        <v>182</v>
+        <v>96</v>
       </c>
       <c r="N19" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O19" s="12">
-        <v>2</v>
-      </c>
-      <c r="P19" s="13">
-        <v>50</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P19" s="13"/>
       <c r="Q19" s="13">
         <f t="shared" ref="Q19" si="18">ROUNDUP(P19*N19,0)</f>
-        <v>50</v>
-      </c>
-      <c r="R19" s="34">
-        <v>4.1000000000000002E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R19" s="34"/>
       <c r="S19" s="34">
         <f t="shared" ref="S19" si="19">R19*Q19</f>
-        <v>2.0500000000000003</v>
+        <v>0</v>
       </c>
       <c r="T19" s="9">
         <f t="shared" si="3"/>
@@ -2508,58 +2443,52 @@
         <v>19</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>154</v>
+        <v>96</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L20" s="12">
-        <v>1844557</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L20" s="12"/>
       <c r="M20" s="33" t="s">
-        <v>183</v>
+        <v>96</v>
       </c>
       <c r="N20" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O20" s="12">
-        <v>4</v>
-      </c>
-      <c r="P20" s="13">
-        <v>100</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P20" s="13"/>
       <c r="Q20" s="13">
         <f>ROUNDUP(P20*N20,0)</f>
-        <v>100</v>
-      </c>
-      <c r="R20" s="34">
-        <v>8.0000000000000002E-3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R20" s="34"/>
       <c r="S20" s="34">
         <f>R20*Q20</f>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="T20" s="9">
         <f>ROW(T20) - ROW($A$1)</f>
@@ -2572,58 +2501,52 @@
         <v>20</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>133</v>
+        <v>96</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>155</v>
+        <v>96</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L21" s="12">
-        <v>45772</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L21" s="12"/>
       <c r="M21" s="33" t="s">
-        <v>184</v>
+        <v>96</v>
       </c>
       <c r="N21" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O21" s="12">
         <v>1</v>
       </c>
-      <c r="P21" s="13">
-        <v>25</v>
-      </c>
+      <c r="P21" s="13"/>
       <c r="Q21" s="13">
         <f t="shared" ref="Q21" si="20">ROUNDUP(P21*N21,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R21" s="34">
-        <v>4.1000000000000002E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R21" s="34"/>
       <c r="S21" s="34">
         <f t="shared" ref="S21" si="21">R21*Q21</f>
-        <v>1.0250000000000001</v>
+        <v>0</v>
       </c>
       <c r="T21" s="9">
         <f t="shared" si="3"/>
@@ -2636,58 +2559,52 @@
         <v>21</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L22" s="12">
-        <v>1232071</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L22" s="12"/>
       <c r="M22" s="33" t="s">
-        <v>185</v>
+        <v>96</v>
       </c>
       <c r="N22" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O22" s="12">
-        <v>2</v>
-      </c>
-      <c r="P22" s="13">
-        <v>50</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P22" s="13"/>
       <c r="Q22" s="13">
         <f>ROUNDUP(P22*N22,0)</f>
-        <v>50</v>
-      </c>
-      <c r="R22" s="34">
-        <v>1.0999999999999999E-2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R22" s="34"/>
       <c r="S22" s="34">
         <f>R22*Q22</f>
-        <v>0.54999999999999993</v>
+        <v>0</v>
       </c>
       <c r="T22" s="9">
         <f>ROW(T22) - ROW($A$1)</f>
@@ -2700,58 +2617,52 @@
         <v>22</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L23" s="12">
-        <v>3171</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L23" s="12"/>
       <c r="M23" s="33" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="N23" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O23" s="12">
-        <v>3</v>
-      </c>
-      <c r="P23" s="13">
-        <v>75</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="P23" s="13"/>
       <c r="Q23" s="13">
         <f t="shared" ref="Q23" si="22">ROUNDUP(P23*N23,0)</f>
-        <v>75</v>
-      </c>
-      <c r="R23" s="34">
-        <v>0.58899999999999997</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R23" s="34"/>
       <c r="S23" s="34">
         <f t="shared" ref="S23" si="23">R23*Q23</f>
-        <v>44.174999999999997</v>
+        <v>0</v>
       </c>
       <c r="T23" s="9">
         <f t="shared" si="3"/>
@@ -2764,58 +2675,52 @@
         <v>23</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L24" s="12">
-        <v>12647</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L24" s="12"/>
       <c r="M24" s="33" t="s">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="N24" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O24" s="12">
         <v>1</v>
       </c>
-      <c r="P24" s="13">
-        <v>25</v>
-      </c>
+      <c r="P24" s="13"/>
       <c r="Q24" s="13">
         <f>ROUNDUP(P24*N24,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R24" s="34">
-        <v>0.63800000000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R24" s="34"/>
       <c r="S24" s="34">
         <f>R24*Q24</f>
-        <v>15.950000000000001</v>
+        <v>0</v>
       </c>
       <c r="T24" s="9">
         <f>ROW(T24) - ROW($A$1)</f>
@@ -2828,58 +2733,52 @@
         <v>24</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>158</v>
+        <v>96</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L25" s="12">
-        <v>3650</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L25" s="12"/>
       <c r="M25" s="33" t="s">
-        <v>188</v>
+        <v>96</v>
       </c>
       <c r="N25" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O25" s="12">
         <v>1</v>
       </c>
-      <c r="P25" s="13">
-        <v>25</v>
-      </c>
+      <c r="P25" s="13"/>
       <c r="Q25" s="13">
         <f t="shared" ref="Q25" si="24">ROUNDUP(P25*N25,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R25" s="34">
-        <v>0.82299999999999995</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R25" s="34"/>
       <c r="S25" s="34">
         <f t="shared" ref="S25" si="25">R25*Q25</f>
-        <v>20.574999999999999</v>
+        <v>0</v>
       </c>
       <c r="T25" s="9">
         <f t="shared" si="3"/>
@@ -2892,58 +2791,52 @@
         <v>25</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G26" s="38" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L26" s="12">
-        <v>-4</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L26" s="12"/>
       <c r="M26" s="33" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="N26" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O26" s="12">
         <v>1</v>
       </c>
-      <c r="P26" s="13">
-        <v>25</v>
-      </c>
+      <c r="P26" s="13"/>
       <c r="Q26" s="13">
         <f>ROUNDUP(P26*N26,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R26" s="34">
-        <v>4.92</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R26" s="34"/>
       <c r="S26" s="34">
         <f>R26*Q26</f>
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="T26" s="9">
         <f>ROW(T26) - ROW($A$1)</f>
@@ -2956,58 +2849,52 @@
         <v>26</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="L27" s="12">
-        <v>7840</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L27" s="12"/>
       <c r="M27" s="33" t="s">
-        <v>190</v>
+        <v>96</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O27" s="12">
-        <v>1</v>
-      </c>
-      <c r="P27" s="13">
-        <v>25</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="P27" s="13"/>
       <c r="Q27" s="13">
         <f t="shared" ref="Q27" si="26">ROUNDUP(P27*N27,0)</f>
-        <v>25</v>
-      </c>
-      <c r="R27" s="34">
-        <v>1.34</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R27" s="34"/>
       <c r="S27" s="34">
         <f t="shared" ref="S27" si="27">R27*Q27</f>
-        <v>33.5</v>
+        <v>0</v>
       </c>
       <c r="T27" s="9">
         <f t="shared" si="3"/>
@@ -3020,39 +2907,39 @@
         <v>27</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L28" s="12"/>
       <c r="M28" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N28" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O28" s="12">
         <v>1</v>
@@ -3078,42 +2965,42 @@
         <v>28</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L29" s="12"/>
       <c r="M29" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N29" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O29" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="13">
@@ -3136,39 +3023,39 @@
         <v>29</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L30" s="12"/>
       <c r="M30" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N30" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O30" s="12">
         <v>1</v>
@@ -3194,39 +3081,39 @@
         <v>30</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G31" s="38" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L31" s="12"/>
       <c r="M31" s="33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N31" s="47" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="O31" s="12">
         <v>1</v>
@@ -3267,23 +3154,23 @@
       <c r="R32" s="23"/>
       <c r="S32" s="23"/>
     </row>
-    <row r="33" spans="1:19" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="15"/>
-      <c r="C33" s="48" t="s">
-        <v>9</v>
+      <c r="C33" s="50" t="s">
+        <v>10</v>
       </c>
       <c r="E33" s="19"/>
       <c r="F33" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G33" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="48" t="s">
+      <c r="G33" s="51" t="s">
         <v>11</v>
+      </c>
+      <c r="H33" s="50" t="s">
+        <v>12</v>
       </c>
       <c r="I33" s="19"/>
       <c r="K33" s="16" t="s">
@@ -3292,7 +3179,7 @@
       <c r="L33" s="17"/>
       <c r="M33" s="39">
         <f ca="1">NOW()</f>
-        <v>42296.446042824071</v>
+        <v>42296.476466087966</v>
       </c>
       <c r="N33" s="45"/>
       <c r="O33" s="18"/>
@@ -3303,25 +3190,32 @@
       </c>
       <c r="S33" s="41">
         <f>SUM(S2:S31)</f>
-        <v>400.42500000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>367.02499999999998</v>
+      </c>
+      <c r="T33" s="49">
+        <f>(SUM(T2:T31))/P34</f>
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M34" s="25" t="s">
         <v>4</v>
       </c>
       <c r="N34" s="46"/>
       <c r="O34" s="35"/>
-      <c r="P34" s="50" t="s">
-        <v>12</v>
+      <c r="P34" s="52" t="s">
+        <v>13</v>
       </c>
       <c r="Q34" s="44"/>
       <c r="R34" s="42"/>
       <c r="S34" s="43" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="T34" s="48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update suppliers fields make mouser basket, reqForms for 20pcb+25parts signed
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="200">
   <si>
     <t>Item #</t>
   </si>
@@ -52,7 +52,7 @@
     <t>19/10/2015</t>
   </si>
   <si>
-    <t>11:25:59</t>
+    <t>14:57:14</t>
   </si>
   <si>
     <t>25</t>
@@ -67,7 +67,13 @@
     <t>C11</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C12</t>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C12, C15</t>
+  </si>
+  <si>
+    <t>C6</t>
   </si>
   <si>
     <t>C7, C9</t>
@@ -76,10 +82,7 @@
     <t>C8, C10</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2, D3, D4, D5, D6, D7</t>
+    <t>D1, D2, D3, D4, D5, D6, D7</t>
   </si>
   <si>
     <t>JP1</t>
@@ -88,7 +91,28 @@
     <t>JP2</t>
   </si>
   <si>
-    <t>R3, R4, R8, R13</t>
+    <t>JP6, JP7</t>
+  </si>
+  <si>
+    <t>LD1</t>
+  </si>
+  <si>
+    <t>LD2</t>
+  </si>
+  <si>
+    <t>LD3</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R7, R8, R13</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R6</t>
   </si>
   <si>
     <t>R9, R10</t>
@@ -97,57 +121,27 @@
     <t>SW1, SW2, SW3</t>
   </si>
   <si>
+    <t>U1</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
     <t>Y1</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
     <t>Y2</t>
   </si>
   <si>
     <t>B2</t>
   </si>
   <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>JP3</t>
   </si>
   <si>
     <t>JP4</t>
   </si>
   <si>
-    <t>LD1</t>
-  </si>
-  <si>
-    <t>LD2</t>
-  </si>
-  <si>
-    <t>LD3</t>
-  </si>
-  <si>
-    <t>R1, R2, R5, R7</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12, R14</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -160,10 +154,16 @@
     <t>0.011F</t>
   </si>
   <si>
+    <t>10uF/MLCC</t>
+  </si>
+  <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>7pF</t>
+    <t>18pF</t>
+  </si>
+  <si>
+    <t>6.8pF</t>
   </si>
   <si>
     <t>1uF/MLCC</t>
@@ -178,60 +178,57 @@
     <t>Header 5X2 1.27mm</t>
   </si>
   <si>
+    <t>HEADER 9</t>
+  </si>
+  <si>
+    <t>LED_RED</t>
+  </si>
+  <si>
+    <t>LED_GRN</t>
+  </si>
+  <si>
+    <t>LED_BLU</t>
+  </si>
+  <si>
     <t>10K</t>
   </si>
   <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>680R</t>
+  </si>
+  <si>
+    <t>18K</t>
+  </si>
+  <si>
     <t>0R</t>
   </si>
   <si>
     <t>EVQ-P2202M</t>
   </si>
   <si>
+    <t>LPC11U68JBD48</t>
+  </si>
+  <si>
     <t>TPS78233</t>
   </si>
   <si>
     <t>FC135-32.76KAA3</t>
   </si>
   <si>
-    <t>LPC11U68JBD48</t>
-  </si>
-  <si>
     <t>12MHz/10pF</t>
   </si>
   <si>
     <t>N-GMS</t>
   </si>
   <si>
-    <t>10uF/MLCC</t>
-  </si>
-  <si>
-    <t>18pF</t>
-  </si>
-  <si>
     <t>HEADER-2</t>
   </si>
   <si>
     <t>HEADER_5</t>
   </si>
   <si>
-    <t>LED_RED</t>
-  </si>
-  <si>
-    <t>LED_GRN</t>
-  </si>
-  <si>
-    <t>LED_BLU</t>
-  </si>
-  <si>
-    <t>620R</t>
-  </si>
-  <si>
-    <t>470R</t>
-  </si>
-  <si>
-    <t>18K</t>
-  </si>
-  <si>
     <t>N-NODE24-20pin</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>0603_CAP</t>
   </si>
   <si>
-    <t>0603_DIODE-CASE_152AB</t>
-  </si>
-  <si>
     <t>0603_DIODE-CDSU101A</t>
   </si>
   <si>
@@ -259,21 +253,33 @@
     <t>2x5-1.27mm-HARWIN-855-M50-3600542</t>
   </si>
   <si>
+    <t>1X12-NOSILK</t>
+  </si>
+  <si>
+    <t>0603_LED_RED</t>
+  </si>
+  <si>
+    <t>0603_LED_GRN</t>
+  </si>
+  <si>
+    <t>0603_LED_BLU</t>
+  </si>
+  <si>
     <t>0603_res</t>
   </si>
   <si>
     <t>BUTTON_4.7x3.5mm</t>
   </si>
   <si>
+    <t>SOT313-2_V</t>
+  </si>
+  <si>
     <t>SOT23-5_0.95mm-NOSILK</t>
   </si>
   <si>
     <t>CRYSTAL-3.2x1.5</t>
   </si>
   <si>
-    <t>SOT313-2_V</t>
-  </si>
-  <si>
     <t>CRY-SMD4-EPSON-FA238V</t>
   </si>
   <si>
@@ -283,15 +289,6 @@
     <t>1X05</t>
   </si>
   <si>
-    <t>0603_LED_RED</t>
-  </si>
-  <si>
-    <t>0603_LED_GRN</t>
-  </si>
-  <si>
-    <t>0603_LED_BLU</t>
-  </si>
-  <si>
     <t>N-NODE24-20pins</t>
   </si>
   <si>
@@ -331,9 +328,18 @@
     <t>Supercapacitors / Ultracapacitors SUPER CAP 3.3V 0.011F</t>
   </si>
   <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 10uF 10volts X5R + - 10%</t>
+  </si>
+  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 0.1uF 10% X7R</t>
   </si>
   <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 25volts 18pF 2% C0G</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 200volts 6.8pF ULTRA LOW ESR</t>
+  </si>
+  <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 1.0uF 16volts X7R 10%</t>
   </si>
   <si>
@@ -346,25 +352,46 @@
     <t>Headers &amp; Wire Housings 5+5 DIL PIN HDR SMT Au/Sn</t>
   </si>
   <si>
+    <t>Headers &amp; Wire Housings 50P SINGLE ROW</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD Super Red, 630nm 17mcd, 2mA</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD Green, 570nm 10mcd, 2mA</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD Blue, 470nm 45mcd, 5mA</t>
+  </si>
+  <si>
     <t>Thick Film Resistors - SMD 0603 10Kohms 1% Tol</t>
   </si>
   <si>
+    <t>Thick Film Resistors - SMD 0603 1Kohms 1% Tol</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 1/10watt 680ohms 1%</t>
+  </si>
+  <si>
+    <t>Thick Film Resistors - SMD 0603 118Kohms 1% Tol</t>
+  </si>
+  <si>
     <t>Thick Film Resistors - SMD 0603 Zero Ohms</t>
   </si>
   <si>
     <t>Tactile Switches 4.7x3.5mm SMD Light Touch Switch</t>
   </si>
   <si>
+    <t>ARM Microcontrollers - MCU LPC11U68JBD48/LQFP48/STANDARD</t>
+  </si>
+  <si>
     <t>LDO Voltage Regulators Sgl Fixed Out LDO 150mA,1uA Quies Crnt</t>
   </si>
   <si>
     <t>Crystals 32.768KHz 20ppm 12.5pF -40C -85C</t>
   </si>
   <si>
-    <t>NXP - LPC11U68JBD48E - MCU, 32BIT, CORTEX-M0+, 50MHZ, LQFP-48</t>
-  </si>
-  <si>
-    <t>ABRACON - ABM8G-12.000MHZ-B4Y-T - CRYSTAL, 12MHZ, 18PF, SMD</t>
+    <t>Crystals 12.000MHz 10pF 30ppm -20C +70C</t>
   </si>
   <si>
     <t>Manufacturer 1</t>
@@ -388,18 +415,27 @@
     <t>Harwin</t>
   </si>
   <si>
+    <t>TE Connectivity / AMP</t>
+  </si>
+  <si>
+    <t>OSRAM Opto Semiconductors</t>
+  </si>
+  <si>
     <t>Panasonic</t>
   </si>
   <si>
+    <t>Vishay / Dale</t>
+  </si>
+  <si>
+    <t>NXP Semiconductors</t>
+  </si>
+  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
     <t>Epson Timing</t>
   </si>
   <si>
-    <t>NXP</t>
-  </si>
-  <si>
     <t>ABRACON</t>
   </si>
   <si>
@@ -412,9 +448,18 @@
     <t>PAS3225P3R3113</t>
   </si>
   <si>
+    <t>GRM188R61A106KE69D</t>
+  </si>
+  <si>
     <t>06035C104KAT2A</t>
   </si>
   <si>
+    <t>02013A180GAT2A</t>
+  </si>
+  <si>
+    <t>06032U6R8BAT2A</t>
+  </si>
+  <si>
     <t>GCM188R71C105KA64D</t>
   </si>
   <si>
@@ -424,21 +469,42 @@
     <t>M50-3600542</t>
   </si>
   <si>
+    <t>5-825433-0</t>
+  </si>
+  <si>
+    <t>LS L29K-G1J2-1-Z</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24-Z</t>
+  </si>
+  <si>
+    <t>LB Q39G-L2N2-35-1</t>
+  </si>
+  <si>
     <t>ERJ-3EKF1002V</t>
   </si>
   <si>
+    <t>ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t>CRCW0603680RFKEA</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1183V</t>
+  </si>
+  <si>
     <t>ERJ-3GEY0R00V</t>
   </si>
   <si>
+    <t>LPC11U68JBD48E</t>
+  </si>
+  <si>
     <t>TPS78233DDCR</t>
   </si>
   <si>
     <t>FC-135 32.7680KA-A3</t>
   </si>
   <si>
-    <t>LPC11U68JBD48E</t>
-  </si>
-  <si>
     <t>ABM8G-12.000MHZ-B4Y-T</t>
   </si>
   <si>
@@ -448,9 +514,6 @@
     <t>Mouser</t>
   </si>
   <si>
-    <t>Farnell</t>
-  </si>
-  <si>
     <t>Supplier Currency 1</t>
   </si>
   <si>
@@ -469,9 +532,18 @@
     <t>963-PAS3225P3R3113</t>
   </si>
   <si>
+    <t>81-GRM188R61A106KE9D</t>
+  </si>
+  <si>
     <t>581-06035C104KAT2A</t>
   </si>
   <si>
+    <t>581-02013A180GAT2A</t>
+  </si>
+  <si>
+    <t>581-06032U6R8BAT2A</t>
+  </si>
+  <si>
     <t>81-GCM188R71C105K64D</t>
   </si>
   <si>
@@ -484,31 +556,55 @@
     <t>855-M50-3600542</t>
   </si>
   <si>
+    <t>571-5-825433-0</t>
+  </si>
+  <si>
+    <t>720-LSL29K-G1J2-1-Z</t>
+  </si>
+  <si>
+    <t>720-LGL29KF2J124Z</t>
+  </si>
+  <si>
+    <t>720-LBQ39GL2N2351</t>
+  </si>
+  <si>
     <t>667-ERJ-3EKF1002V</t>
   </si>
   <si>
+    <t>667-ERJ-3EKF1001V</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-680-E3</t>
+  </si>
+  <si>
+    <t>667-ERJ-3EKF1183V</t>
+  </si>
+  <si>
     <t>667-ERJ-3GEY0R00V</t>
   </si>
   <si>
     <t>667-EVQ-P2202M</t>
   </si>
   <si>
+    <t>771-LPC11U68JBD48E</t>
+  </si>
+  <si>
     <t>595-TPS78233DDCR</t>
   </si>
   <si>
     <t>732-FC135-32.76KAA3</t>
   </si>
   <si>
-    <t>2433462</t>
-  </si>
-  <si>
-    <t>2308707</t>
+    <t>815-ABM8G-12-B4Y-T</t>
   </si>
   <si>
     <t>Divider</t>
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>0.25</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -1207,7 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T35"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
@@ -1243,52 +1342,52 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>94</v>
-      </c>
       <c r="G1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>8</v>
@@ -1306,38 +1405,38 @@
         <v>15</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L2" s="12">
         <v>210123</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="N2" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O2" s="12">
         <v>1</v>
@@ -1363,45 +1462,45 @@
     </row>
     <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
-        <f t="shared" ref="A3:A31" si="0">ROW(A3) - ROW($A$1)</f>
+        <f t="shared" ref="A3:A29" si="0">ROW(A3) - ROW($A$1)</f>
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L3" s="12">
         <v>6237</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="N3" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O3" s="12">
         <v>1</v>
@@ -1410,18 +1509,18 @@
         <v>25</v>
       </c>
       <c r="Q3" s="13">
-        <f t="shared" ref="Q3:Q31" si="1">ROUNDUP(P3*N3,0)</f>
+        <f t="shared" ref="Q3:Q29" si="1">ROUNDUP(P3*N3,0)</f>
         <v>25</v>
       </c>
       <c r="R3" s="34">
         <v>1.6</v>
       </c>
       <c r="S3" s="34">
-        <f t="shared" ref="S3:S31" si="2">R3*Q3</f>
+        <f t="shared" ref="S3:S29" si="2">R3*Q3</f>
         <v>40</v>
       </c>
       <c r="T3" s="9">
-        <f t="shared" ref="T3:T31" si="3">ROW(T3) - ROW($A$1)</f>
+        <f t="shared" ref="T3:T29" si="3">ROW(T3) - ROW($A$1)</f>
         <v>2</v>
       </c>
     </row>
@@ -1434,55 +1533,55 @@
         <v>17</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L4" s="12">
-        <v>483363</v>
+        <v>306957</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="N4" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O4" s="12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P4" s="13">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="13">
         <f>ROUNDUP(P4*N4,0)</f>
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="R4" s="34">
-        <v>2.7E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="S4" s="34">
         <f>R4*Q4</f>
-        <v>3.375</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="T4" s="9">
         <f>ROW(T4) - ROW($A$1)</f>
@@ -1498,55 +1597,55 @@
         <v>18</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L5" s="12">
-        <v>210123</v>
+        <v>483187</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="N5" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O5" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P5" s="13">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="13">
         <f t="shared" ref="Q5" si="4">ROUNDUP(P5*N5,0)</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="R5" s="34">
-        <v>0.03</v>
+        <v>2.7E-2</v>
       </c>
       <c r="S5" s="34">
         <f t="shared" ref="S5" si="5">R5*Q5</f>
-        <v>1.5</v>
+        <v>4.05</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" si="3"/>
@@ -1562,55 +1661,55 @@
         <v>19</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G6" s="38" t="s">
         <v>106</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L6" s="12">
-        <v>197098</v>
+        <v>28018</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="N6" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O6" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6" s="13">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="Q6" s="13">
         <f>ROUNDUP(P6*N6,0)</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="R6" s="34">
-        <v>0.151</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="S6" s="34">
         <f>R6*Q6</f>
-        <v>7.55</v>
+        <v>2.2749999999999999</v>
       </c>
       <c r="T6" s="9">
         <f>ROW(T6) - ROW($A$1)</f>
@@ -1626,55 +1725,55 @@
         <v>20</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G7" s="38" t="s">
         <v>107</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L7" s="12">
-        <v>32441</v>
+        <v>22521</v>
       </c>
       <c r="M7" s="33" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="N7" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O7" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P7" s="13">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q7" s="13">
         <f t="shared" ref="Q7" si="6">ROUNDUP(P7*N7,0)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="R7" s="34">
-        <v>0.33500000000000002</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="S7" s="34">
         <f t="shared" ref="S7" si="7">R7*Q7</f>
-        <v>8.375</v>
+        <v>4.55</v>
       </c>
       <c r="T7" s="9">
         <f t="shared" si="3"/>
@@ -1690,55 +1789,55 @@
         <v>21</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L8" s="12">
-        <v>32441</v>
+        <v>197098</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="N8" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O8" s="12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P8" s="13">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="13">
         <f>ROUNDUP(P8*N8,0)</f>
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="R8" s="34">
-        <v>0.186</v>
+        <v>0.151</v>
       </c>
       <c r="S8" s="34">
         <f>R8*Q8</f>
-        <v>27.9</v>
+        <v>7.55</v>
       </c>
       <c r="T8" s="9">
         <f>ROW(T8) - ROW($A$1)</f>
@@ -1754,55 +1853,55 @@
         <v>22</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
         <v>96</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>134</v>
+        <v>51</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L9" s="12">
-        <v>8920</v>
+        <v>32441</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="N9" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O9" s="12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="P9" s="13">
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="Q9" s="13">
         <f t="shared" ref="Q9" si="8">ROUNDUP(P9*N9,0)</f>
-        <v>25</v>
+        <v>175</v>
       </c>
       <c r="R9" s="34">
-        <v>0.68700000000000006</v>
+        <v>0.186</v>
       </c>
       <c r="S9" s="34">
         <f t="shared" ref="S9" si="9">R9*Q9</f>
-        <v>17.175000000000001</v>
+        <v>32.549999999999997</v>
       </c>
       <c r="T9" s="9">
         <f t="shared" si="3"/>
@@ -1818,38 +1917,38 @@
         <v>23</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L10" s="12">
-        <v>9321</v>
+        <v>8920</v>
       </c>
       <c r="M10" s="33" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
       <c r="N10" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O10" s="12">
         <v>1</v>
@@ -1862,11 +1961,11 @@
         <v>25</v>
       </c>
       <c r="R10" s="34">
-        <v>0.874</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="S10" s="34">
         <f>R10*Q10</f>
-        <v>21.85</v>
+        <v>17.175000000000001</v>
       </c>
       <c r="T10" s="9">
         <f>ROW(T10) - ROW($A$1)</f>
@@ -1882,55 +1981,55 @@
         <v>24</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L11" s="12">
-        <v>1844557</v>
+        <v>10009</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="N11" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O11" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P11" s="13">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="13">
         <f t="shared" ref="Q11" si="10">ROUNDUP(P11*N11,0)</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="R11" s="34">
-        <v>8.0000000000000002E-3</v>
+        <v>0.874</v>
       </c>
       <c r="S11" s="34">
         <f t="shared" ref="S11" si="11">R11*Q11</f>
-        <v>0.8</v>
+        <v>21.85</v>
       </c>
       <c r="T11" s="9">
         <f t="shared" si="3"/>
@@ -1946,38 +2045,38 @@
         <v>25</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L12" s="12">
-        <v>1232071</v>
+        <v>37</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="N12" s="47" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="O12" s="12">
         <v>2</v>
@@ -1987,14 +2086,14 @@
       </c>
       <c r="Q12" s="13">
         <f>ROUNDUP(P12*N12,0)</f>
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="R12" s="34">
-        <v>1.0999999999999999E-2</v>
+        <v>2.83</v>
       </c>
       <c r="S12" s="34">
         <f>R12*Q12</f>
-        <v>0.54999999999999993</v>
+        <v>36.79</v>
       </c>
       <c r="T12" s="9">
         <f>ROW(T12) - ROW($A$1)</f>
@@ -2010,55 +2109,55 @@
         <v>26</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L13" s="12">
-        <v>3171</v>
+        <v>74824</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
       <c r="N13" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O13" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P13" s="13">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="Q13" s="13">
         <f t="shared" ref="Q13" si="12">ROUNDUP(P13*N13,0)</f>
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="R13" s="34">
-        <v>0.58899999999999997</v>
+        <v>0.108</v>
       </c>
       <c r="S13" s="34">
         <f t="shared" ref="S13" si="13">R13*Q13</f>
-        <v>44.174999999999997</v>
+        <v>2.7</v>
       </c>
       <c r="T13" s="9">
         <f t="shared" si="3"/>
@@ -2074,38 +2173,38 @@
         <v>27</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L14" s="12">
-        <v>12597</v>
+        <v>31893</v>
       </c>
       <c r="M14" s="33" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="N14" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O14" s="12">
         <v>1</v>
@@ -2118,11 +2217,11 @@
         <v>25</v>
       </c>
       <c r="R14" s="34">
-        <v>0.63800000000000001</v>
+        <v>0.108</v>
       </c>
       <c r="S14" s="34">
         <f>R14*Q14</f>
-        <v>15.950000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="T14" s="9">
         <f>ROW(T14) - ROW($A$1)</f>
@@ -2138,38 +2237,38 @@
         <v>28</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L15" s="12">
-        <v>3650</v>
+        <v>109541</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="N15" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O15" s="12">
         <v>1</v>
@@ -2182,11 +2281,11 @@
         <v>25</v>
       </c>
       <c r="R15" s="34">
-        <v>0.82299999999999995</v>
+        <v>0.108</v>
       </c>
       <c r="S15" s="34">
         <f t="shared" ref="S15" si="15">R15*Q15</f>
-        <v>20.574999999999999</v>
+        <v>2.7</v>
       </c>
       <c r="T15" s="9">
         <f t="shared" si="3"/>
@@ -2202,55 +2301,55 @@
         <v>29</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L16" s="12">
-        <v>-4</v>
+        <v>1844557</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="N16" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O16" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="P16" s="13">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="Q16" s="13">
         <f>ROUNDUP(P16*N16,0)</f>
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="R16" s="34">
-        <v>4.92</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="S16" s="34">
         <f>R16*Q16</f>
-        <v>123</v>
+        <v>1.6</v>
       </c>
       <c r="T16" s="9">
         <f>ROW(T16) - ROW($A$1)</f>
@@ -2266,55 +2365,55 @@
         <v>30</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="L17" s="12">
-        <v>7840</v>
+        <v>828858</v>
       </c>
       <c r="M17" s="33" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="N17" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O17" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="13">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="13">
         <f t="shared" ref="Q17" si="16">ROUNDUP(P17*N17,0)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="R17" s="34">
-        <v>1.34</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="S17" s="34">
         <f t="shared" ref="S17" si="17">R17*Q17</f>
-        <v>33.5</v>
+        <v>0.65</v>
       </c>
       <c r="T17" s="9">
         <f t="shared" si="3"/>
@@ -2330,49 +2429,55 @@
         <v>31</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="36" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L18" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L18" s="12">
+        <v>136009</v>
+      </c>
       <c r="M18" s="33" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="N18" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O18" s="12">
         <v>1</v>
       </c>
-      <c r="P18" s="13"/>
+      <c r="P18" s="13">
+        <v>25</v>
+      </c>
       <c r="Q18" s="13">
         <f>ROUNDUP(P18*N18,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R18" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R18" s="34">
+        <v>0.04</v>
+      </c>
       <c r="S18" s="34">
         <f>R18*Q18</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="9">
         <f>ROW(T18) - ROW($A$1)</f>
@@ -2388,49 +2493,55 @@
         <v>32</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L19" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L19" s="12">
+        <v>92176</v>
+      </c>
       <c r="M19" s="33" t="s">
-        <v>96</v>
+        <v>187</v>
       </c>
       <c r="N19" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O19" s="12">
         <v>1</v>
       </c>
-      <c r="P19" s="13"/>
+      <c r="P19" s="13">
+        <v>25</v>
+      </c>
       <c r="Q19" s="13">
         <f t="shared" ref="Q19" si="18">ROUNDUP(P19*N19,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R19" s="34">
+        <v>1.4E-2</v>
+      </c>
       <c r="S19" s="34">
         <f t="shared" ref="S19" si="19">R19*Q19</f>
-        <v>0</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="T19" s="9">
         <f t="shared" si="3"/>
@@ -2446,49 +2557,55 @@
         <v>33</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L20" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L20" s="12">
+        <v>1231971</v>
+      </c>
       <c r="M20" s="33" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="N20" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O20" s="12">
-        <v>1</v>
-      </c>
-      <c r="P20" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="P20" s="13">
+        <v>50</v>
+      </c>
       <c r="Q20" s="13">
         <f>ROUNDUP(P20*N20,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R20" s="34"/>
+        <v>50</v>
+      </c>
+      <c r="R20" s="34">
+        <v>1.0999999999999999E-2</v>
+      </c>
       <c r="S20" s="34">
         <f>R20*Q20</f>
-        <v>0</v>
+        <v>0.54999999999999993</v>
       </c>
       <c r="T20" s="9">
         <f>ROW(T20) - ROW($A$1)</f>
@@ -2507,46 +2624,52 @@
         <v>63</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L21" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L21" s="12">
+        <v>3171</v>
+      </c>
       <c r="M21" s="33" t="s">
-        <v>96</v>
+        <v>189</v>
       </c>
       <c r="N21" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O21" s="12">
-        <v>1</v>
-      </c>
-      <c r="P21" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="P21" s="13">
+        <v>75</v>
+      </c>
       <c r="Q21" s="13">
         <f t="shared" ref="Q21" si="20">ROUNDUP(P21*N21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="34"/>
+        <v>75</v>
+      </c>
+      <c r="R21" s="34">
+        <v>0.58899999999999997</v>
+      </c>
       <c r="S21" s="34">
         <f t="shared" ref="S21" si="21">R21*Q21</f>
-        <v>0</v>
+        <v>44.174999999999997</v>
       </c>
       <c r="T21" s="9">
         <f t="shared" si="3"/>
@@ -2565,46 +2688,52 @@
         <v>64</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L22" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L22" s="12">
+        <v>256</v>
+      </c>
       <c r="M22" s="33" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="N22" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O22" s="12">
         <v>1</v>
       </c>
-      <c r="P22" s="13"/>
+      <c r="P22" s="13">
+        <v>25</v>
+      </c>
       <c r="Q22" s="13">
         <f>ROUNDUP(P22*N22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R22" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R22" s="34">
+        <v>3.83</v>
+      </c>
       <c r="S22" s="34">
         <f>R22*Q22</f>
-        <v>0</v>
+        <v>95.75</v>
       </c>
       <c r="T22" s="9">
         <f>ROW(T22) - ROW($A$1)</f>
@@ -2623,46 +2752,52 @@
         <v>65</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L23" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L23" s="12">
+        <v>12587</v>
+      </c>
       <c r="M23" s="33" t="s">
-        <v>96</v>
+        <v>191</v>
       </c>
       <c r="N23" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O23" s="12">
         <v>1</v>
       </c>
-      <c r="P23" s="13"/>
+      <c r="P23" s="13">
+        <v>25</v>
+      </c>
       <c r="Q23" s="13">
         <f t="shared" ref="Q23" si="22">ROUNDUP(P23*N23,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R23" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R23" s="34">
+        <v>0.63800000000000001</v>
+      </c>
       <c r="S23" s="34">
         <f t="shared" ref="S23" si="23">R23*Q23</f>
-        <v>0</v>
+        <v>15.950000000000001</v>
       </c>
       <c r="T23" s="9">
         <f t="shared" si="3"/>
@@ -2681,46 +2816,52 @@
         <v>66</v>
       </c>
       <c r="D24" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L24" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L24" s="12">
+        <v>3650</v>
+      </c>
       <c r="M24" s="33" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="N24" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O24" s="12">
         <v>1</v>
       </c>
-      <c r="P24" s="13"/>
+      <c r="P24" s="13">
+        <v>25</v>
+      </c>
       <c r="Q24" s="13">
         <f>ROUNDUP(P24*N24,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R24" s="34">
+        <v>0.82299999999999995</v>
+      </c>
       <c r="S24" s="34">
         <f>R24*Q24</f>
-        <v>0</v>
+        <v>20.574999999999999</v>
       </c>
       <c r="T24" s="9">
         <f>ROW(T24) - ROW($A$1)</f>
@@ -2739,46 +2880,52 @@
         <v>67</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G25" s="38" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L25" s="12"/>
+        <v>167</v>
+      </c>
+      <c r="L25" s="12">
+        <v>9046</v>
+      </c>
       <c r="M25" s="33" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="N25" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O25" s="12">
         <v>1</v>
       </c>
-      <c r="P25" s="13"/>
+      <c r="P25" s="13">
+        <v>25</v>
+      </c>
       <c r="Q25" s="13">
         <f t="shared" ref="Q25" si="24">ROUNDUP(P25*N25,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="R25" s="34">
+        <v>0.73099999999999998</v>
+      </c>
       <c r="S25" s="34">
         <f t="shared" ref="S25" si="25">R25*Q25</f>
-        <v>0</v>
+        <v>18.274999999999999</v>
       </c>
       <c r="T25" s="9">
         <f t="shared" si="3"/>
@@ -2797,33 +2944,33 @@
         <v>68</v>
       </c>
       <c r="D26" s="36" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G26" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J26" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L26" s="12"/>
       <c r="M26" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N26" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O26" s="12">
         <v>1</v>
@@ -2852,39 +2999,39 @@
         <v>40</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L27" s="12"/>
       <c r="M27" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N27" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O27" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P27" s="13"/>
       <c r="Q27" s="13">
@@ -2910,36 +3057,36 @@
         <v>41</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G28" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L28" s="12"/>
       <c r="M28" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N28" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O28" s="12">
         <v>1</v>
@@ -2968,39 +3115,39 @@
         <v>42</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D29" s="36" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J29" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L29" s="12"/>
       <c r="M29" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N29" s="47" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="O29" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P29" s="13"/>
       <c r="Q29" s="13">
@@ -3017,207 +3164,91 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <f>ROW(A30) - ROW($A$1)</f>
-        <v>29</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="N30" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="O30" s="12">
+    <row r="30" spans="1:20" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30"/>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+    </row>
+    <row r="31" spans="1:20" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="19"/>
+      <c r="K31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13">
-        <f>ROUNDUP(P30*N30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="34"/>
-      <c r="S30" s="34">
-        <f>R30*Q30</f>
-        <v>0</v>
-      </c>
-      <c r="T30" s="9">
-        <f>ROW(T30) - ROW($A$1)</f>
-        <v>29</v>
+      <c r="L31" s="17"/>
+      <c r="M31" s="39">
+        <f ca="1">NOW()</f>
+        <v>42296.623160648145</v>
+      </c>
+      <c r="N31" s="45"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="S31" s="41">
+        <f>SUM(S2:S29)</f>
+        <v>376.28999999999991</v>
+      </c>
+      <c r="T31" s="49">
+        <f>(SUM(T2:T29))/P32</f>
+        <v>16.239999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="G31" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="N31" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="O31" s="12">
-        <v>1</v>
-      </c>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13">
-        <f t="shared" ref="Q31" si="30">ROUNDUP(P31*N31,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R31" s="34"/>
-      <c r="S31" s="34">
-        <f t="shared" ref="S31" si="31">R31*Q31</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="9">
-        <f t="shared" si="3"/>
-        <v>30</v>
+    <row r="32" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M32" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" s="46"/>
+      <c r="O32" s="35"/>
+      <c r="P32" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="T32" s="48" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="24"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23"/>
-    </row>
-    <row r="33" spans="1:20" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="51" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="I33" s="19"/>
-      <c r="K33" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L33" s="17"/>
-      <c r="M33" s="39">
-        <f ca="1">NOW()</f>
-        <v>42296.476466087966</v>
-      </c>
-      <c r="N33" s="45"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="S33" s="41">
-        <f>SUM(S2:S31)</f>
-        <v>367.02499999999998</v>
-      </c>
-      <c r="T33" s="49">
-        <f>(SUM(T2:T31))/P34</f>
-        <v>18.600000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M34" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="N34" s="46"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q34" s="44"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="T34" s="48" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
18K(supplier link was 118K)   and 18pF (s. link was 0201) updated supplier links Purchase list and deliverables created
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="201">
   <si>
     <t>Item #</t>
   </si>
@@ -49,10 +49,10 @@
     <t>n-baseU68</t>
   </si>
   <si>
-    <t>19/10/2015</t>
-  </si>
-  <si>
-    <t>14:57:14</t>
+    <t>06/11/2015</t>
+  </si>
+  <si>
+    <t>11:02:31</t>
   </si>
   <si>
     <t>25</t>
@@ -334,7 +334,7 @@
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 0.1uF 10% X7R</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 25volts 18pF 2% C0G</t>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 18pF 50volts C0G 5%</t>
   </si>
   <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 200volts 6.8pF ULTRA LOW ESR</t>
@@ -373,7 +373,7 @@
     <t>Thick Film Resistors - SMD 1/10watt 680ohms 1%</t>
   </si>
   <si>
-    <t>Thick Film Resistors - SMD 0603 118Kohms 1% Tol</t>
+    <t>Thick Film Resistors - SMD 0603 1.8Kohms 5% Tol</t>
   </si>
   <si>
     <t>Thick Film Resistors - SMD 0603 Zero Ohms</t>
@@ -406,6 +406,9 @@
     <t>AVX</t>
   </si>
   <si>
+    <t>TDK</t>
+  </si>
+  <si>
     <t>ON Semiconductor</t>
   </si>
   <si>
@@ -454,7 +457,7 @@
     <t>06035C104KAT2A</t>
   </si>
   <si>
-    <t>02013A180GAT2A</t>
+    <t>C1608C0G1H180J080AA</t>
   </si>
   <si>
     <t>06032U6R8BAT2A</t>
@@ -490,7 +493,7 @@
     <t>CRCW0603680RFKEA</t>
   </si>
   <si>
-    <t>ERJ-3EKF1183V</t>
+    <t>ERJ-3GEYJ182V</t>
   </si>
   <si>
     <t>ERJ-3GEY0R00V</t>
@@ -538,7 +541,7 @@
     <t>581-06035C104KAT2A</t>
   </si>
   <si>
-    <t>581-02013A180GAT2A</t>
+    <t>810-C1608C0G1H180J</t>
   </si>
   <si>
     <t>581-06032U6R8BAT2A</t>
@@ -577,7 +580,7 @@
     <t>71-CRCW0603-680-E3</t>
   </si>
   <si>
-    <t>667-ERJ-3EKF1183V</t>
+    <t>667-ERJ-3GEYJ182V</t>
   </si>
   <si>
     <t>667-ERJ-3GEY0R00V</t>
@@ -624,7 +627,7 @@
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy\ hh:mm"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -706,8 +709,22 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -744,8 +761,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -853,11 +876,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,13 +919,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -946,9 +972,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -990,13 +1013,34 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1308,8 +1352,8 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1322,13 +1366,13 @@
     <col min="7" max="7" width="36.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="27" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="25" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" customWidth="1"/>
     <col min="12" max="12" width="8.140625" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" style="29" customWidth="1"/>
-    <col min="14" max="14" width="4.28515625" style="29" customWidth="1"/>
+    <col min="13" max="13" width="28" style="27" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" style="27" customWidth="1"/>
     <col min="15" max="15" width="5.42578125" style="1" customWidth="1"/>
-    <col min="16" max="17" width="6.42578125" style="32" customWidth="1"/>
+    <col min="16" max="17" width="6.42578125" style="30" customWidth="1"/>
     <col min="18" max="18" width="10.28515625" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
     <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
@@ -1360,39 +1404,39 @@
         <v>126</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Q1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="48" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1401,61 +1445,61 @@
         <f>ROW(A2) - ROW($A$1)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="33" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="G2" s="35" t="s">
         <v>102</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>127</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>165</v>
+        <v>143</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L2" s="12">
-        <v>210123</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O2" s="12">
+        <v>168</v>
+      </c>
+      <c r="L2" s="11">
+        <v>207370</v>
+      </c>
+      <c r="M2" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O2" s="11">
         <v>1</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="47">
         <v>25</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="51">
         <f>ROUNDUP(P2*N2,0)</f>
         <v>25</v>
       </c>
-      <c r="R2" s="34">
+      <c r="R2" s="31">
         <v>0.03</v>
       </c>
-      <c r="S2" s="34">
+      <c r="S2" s="31">
         <f>R2*Q2</f>
         <v>0.75</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="52">
         <f>ROW(T2) - ROW($A$1)</f>
         <v>1</v>
       </c>
@@ -1465,61 +1509,61 @@
         <f t="shared" ref="A3:A29" si="0">ROW(A3) - ROW($A$1)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>74</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>103</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>128</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>165</v>
+        <v>144</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L3" s="12">
-        <v>6237</v>
-      </c>
-      <c r="M3" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="N3" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O3" s="12">
+        <v>168</v>
+      </c>
+      <c r="L3" s="11">
+        <v>2310</v>
+      </c>
+      <c r="M3" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="N3" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O3" s="11">
         <v>1</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="47">
         <v>25</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="51">
         <f t="shared" ref="Q3:Q29" si="1">ROUNDUP(P3*N3,0)</f>
         <v>25</v>
       </c>
-      <c r="R3" s="34">
+      <c r="R3" s="31">
         <v>1.6</v>
       </c>
-      <c r="S3" s="34">
+      <c r="S3" s="31">
         <f t="shared" ref="S3:S29" si="2">R3*Q3</f>
         <v>40</v>
       </c>
-      <c r="T3" s="9">
+      <c r="T3" s="52">
         <f t="shared" ref="T3:T29" si="3">ROW(T3) - ROW($A$1)</f>
         <v>2</v>
       </c>
@@ -1529,61 +1573,61 @@
         <f>ROW(A4) - ROW($A$1)</f>
         <v>3</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="33" t="s">
         <v>75</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="35" t="s">
         <v>104</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>127</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>165</v>
+        <v>145</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L4" s="12">
-        <v>306957</v>
-      </c>
-      <c r="M4" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="N4" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O4" s="12">
+        <v>168</v>
+      </c>
+      <c r="L4" s="11">
+        <v>237021</v>
+      </c>
+      <c r="M4" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O4" s="11">
         <v>1</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="47">
         <v>25</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="51">
         <f>ROUNDUP(P4*N4,0)</f>
         <v>25</v>
       </c>
-      <c r="R4" s="34">
+      <c r="R4" s="31">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="S4" s="34">
+      <c r="S4" s="31">
         <f>R4*Q4</f>
         <v>1.7749999999999999</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="52">
         <f>ROW(T4) - ROW($A$1)</f>
         <v>3</v>
       </c>
@@ -1593,61 +1637,61 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="35" t="s">
         <v>105</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>129</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>165</v>
+        <v>146</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L5" s="12">
-        <v>483187</v>
-      </c>
-      <c r="M5" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="N5" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O5" s="12">
+        <v>168</v>
+      </c>
+      <c r="L5" s="11">
+        <v>448558</v>
+      </c>
+      <c r="M5" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O5" s="11">
         <v>6</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="47">
         <v>150</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="51">
         <f t="shared" ref="Q5" si="4">ROUNDUP(P5*N5,0)</f>
         <v>150</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="31">
         <v>2.7E-2</v>
       </c>
-      <c r="S5" s="34">
+      <c r="S5" s="31">
         <f t="shared" ref="S5" si="5">R5*Q5</f>
         <v>4.05</v>
       </c>
-      <c r="T5" s="9">
+      <c r="T5" s="52">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
@@ -1657,61 +1701,61 @@
         <f>ROW(A6) - ROW($A$1)</f>
         <v>5</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="35" t="s">
         <v>106</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>165</v>
+        <v>147</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L6" s="12">
-        <v>28018</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O6" s="12">
+        <v>168</v>
+      </c>
+      <c r="L6" s="11">
+        <v>53490</v>
+      </c>
+      <c r="M6" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="N6" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O6" s="11">
         <v>1</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="47">
         <v>25</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="51">
         <f>ROUNDUP(P6*N6,0)</f>
         <v>25</v>
       </c>
-      <c r="R6" s="34">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="S6" s="34">
+      <c r="R6" s="31">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="S6" s="31">
         <f>R6*Q6</f>
-        <v>2.2749999999999999</v>
-      </c>
-      <c r="T6" s="9">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="T6" s="52">
         <f>ROW(T6) - ROW($A$1)</f>
         <v>5</v>
       </c>
@@ -1721,61 +1765,61 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="33" t="s">
         <v>73</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="35" t="s">
         <v>107</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>129</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>165</v>
+        <v>148</v>
+      </c>
+      <c r="J7" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L7" s="12">
-        <v>22521</v>
-      </c>
-      <c r="M7" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="N7" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O7" s="12">
+        <v>168</v>
+      </c>
+      <c r="L7" s="11">
+        <v>22321</v>
+      </c>
+      <c r="M7" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O7" s="11">
         <v>2</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="47">
         <v>50</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="51">
         <f t="shared" ref="Q7" si="6">ROUNDUP(P7*N7,0)</f>
         <v>50</v>
       </c>
-      <c r="R7" s="34">
+      <c r="R7" s="31">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="S7" s="34">
+      <c r="S7" s="31">
         <f t="shared" ref="S7" si="7">R7*Q7</f>
         <v>4.55</v>
       </c>
-      <c r="T7" s="9">
+      <c r="T7" s="52">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -1785,61 +1829,61 @@
         <f>ROW(A8) - ROW($A$1)</f>
         <v>7</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>75</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="35" t="s">
         <v>108</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>127</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>165</v>
+        <v>149</v>
+      </c>
+      <c r="J8" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L8" s="12">
-        <v>197098</v>
-      </c>
-      <c r="M8" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="N8" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O8" s="12">
+        <v>168</v>
+      </c>
+      <c r="L8" s="11">
+        <v>193349</v>
+      </c>
+      <c r="M8" s="50" t="s">
+        <v>177</v>
+      </c>
+      <c r="N8" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O8" s="11">
         <v>2</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="47">
         <v>50</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="51">
         <f>ROUNDUP(P8*N8,0)</f>
         <v>50</v>
       </c>
-      <c r="R8" s="34">
-        <v>0.151</v>
-      </c>
-      <c r="S8" s="34">
+      <c r="R8" s="31">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="S8" s="31">
         <f>R8*Q8</f>
-        <v>7.55</v>
-      </c>
-      <c r="T8" s="9">
+        <v>5.8500000000000005</v>
+      </c>
+      <c r="T8" s="52">
         <f>ROW(T8) - ROW($A$1)</f>
         <v>7</v>
       </c>
@@ -1849,61 +1893,61 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="33" t="s">
         <v>76</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="35" t="s">
         <v>109</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>165</v>
+      <c r="J9" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L9" s="12">
-        <v>32441</v>
-      </c>
-      <c r="M9" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="N9" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O9" s="12">
+        <v>168</v>
+      </c>
+      <c r="L9" s="11">
+        <v>29471</v>
+      </c>
+      <c r="M9" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="N9" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O9" s="11">
         <v>7</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="47">
         <v>175</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="51">
         <f t="shared" ref="Q9" si="8">ROUNDUP(P9*N9,0)</f>
         <v>175</v>
       </c>
-      <c r="R9" s="34">
-        <v>0.186</v>
-      </c>
-      <c r="S9" s="34">
+      <c r="R9" s="31">
+        <v>0.192</v>
+      </c>
+      <c r="S9" s="31">
         <f t="shared" ref="S9" si="9">R9*Q9</f>
-        <v>32.549999999999997</v>
-      </c>
-      <c r="T9" s="9">
+        <v>33.6</v>
+      </c>
+      <c r="T9" s="52">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -1913,61 +1957,61 @@
         <f>ROW(A10) - ROW($A$1)</f>
         <v>9</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="33" t="s">
         <v>77</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="35" t="s">
         <v>110</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>165</v>
+        <v>150</v>
+      </c>
+      <c r="J10" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L10" s="12">
-        <v>8920</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="N10" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O10" s="12">
+        <v>168</v>
+      </c>
+      <c r="L10" s="11">
+        <v>7383</v>
+      </c>
+      <c r="M10" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="N10" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O10" s="11">
         <v>1</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="47">
         <v>25</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="51">
         <f>ROUNDUP(P10*N10,0)</f>
         <v>25</v>
       </c>
-      <c r="R10" s="34">
+      <c r="R10" s="31">
         <v>0.68700000000000006</v>
       </c>
-      <c r="S10" s="34">
+      <c r="S10" s="31">
         <f>R10*Q10</f>
         <v>17.175000000000001</v>
       </c>
-      <c r="T10" s="9">
+      <c r="T10" s="52">
         <f>ROW(T10) - ROW($A$1)</f>
         <v>9</v>
       </c>
@@ -1977,61 +2021,61 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="33" t="s">
         <v>78</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="35" t="s">
         <v>111</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>165</v>
+        <v>151</v>
+      </c>
+      <c r="J11" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L11" s="12">
-        <v>10009</v>
-      </c>
-      <c r="M11" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="N11" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O11" s="12">
+        <v>168</v>
+      </c>
+      <c r="L11" s="11">
+        <v>8817</v>
+      </c>
+      <c r="M11" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O11" s="11">
         <v>1</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="47">
         <v>25</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="51">
         <f t="shared" ref="Q11" si="10">ROUNDUP(P11*N11,0)</f>
         <v>25</v>
       </c>
-      <c r="R11" s="34">
+      <c r="R11" s="31">
         <v>0.874</v>
       </c>
-      <c r="S11" s="34">
+      <c r="S11" s="31">
         <f t="shared" ref="S11" si="11">R11*Q11</f>
         <v>21.85</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11" s="52">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -2041,61 +2085,61 @@
         <f>ROW(A12) - ROW($A$1)</f>
         <v>11</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="33" t="s">
         <v>79</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="35" t="s">
         <v>112</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>165</v>
+        <v>152</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L12" s="12">
-        <v>37</v>
-      </c>
-      <c r="M12" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="N12" s="47" t="s">
-        <v>196</v>
-      </c>
-      <c r="O12" s="12">
+        <v>168</v>
+      </c>
+      <c r="L12" s="11">
+        <v>298</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="O12" s="11">
         <v>2</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="47">
         <v>50</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="51">
         <f>ROUNDUP(P12*N12,0)</f>
         <v>13</v>
       </c>
-      <c r="R12" s="34">
+      <c r="R12" s="31">
         <v>2.83</v>
       </c>
-      <c r="S12" s="34">
+      <c r="S12" s="31">
         <f>R12*Q12</f>
         <v>36.79</v>
       </c>
-      <c r="T12" s="9">
+      <c r="T12" s="52">
         <f>ROW(T12) - ROW($A$1)</f>
         <v>11</v>
       </c>
@@ -2105,61 +2149,61 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="33" t="s">
         <v>80</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="35" t="s">
         <v>113</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>165</v>
+        <v>153</v>
+      </c>
+      <c r="J13" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L13" s="12">
-        <v>74824</v>
-      </c>
-      <c r="M13" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="N13" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O13" s="12">
+        <v>168</v>
+      </c>
+      <c r="L13" s="11">
+        <v>63048</v>
+      </c>
+      <c r="M13" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="N13" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O13" s="11">
         <v>1</v>
       </c>
-      <c r="P13" s="13">
+      <c r="P13" s="47">
         <v>25</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="51">
         <f t="shared" ref="Q13" si="12">ROUNDUP(P13*N13,0)</f>
         <v>25</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="31">
         <v>0.108</v>
       </c>
-      <c r="S13" s="34">
+      <c r="S13" s="31">
         <f t="shared" ref="S13" si="13">R13*Q13</f>
         <v>2.7</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13" s="52">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -2169,61 +2213,61 @@
         <f>ROW(A14) - ROW($A$1)</f>
         <v>13</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="33" t="s">
         <v>81</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="35" t="s">
         <v>114</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>165</v>
+        <v>154</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L14" s="12">
-        <v>31893</v>
-      </c>
-      <c r="M14" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="N14" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O14" s="12">
+        <v>168</v>
+      </c>
+      <c r="L14" s="11">
+        <v>43058</v>
+      </c>
+      <c r="M14" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="N14" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O14" s="11">
         <v>1</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="47">
         <v>25</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="51">
         <f>ROUNDUP(P14*N14,0)</f>
         <v>25</v>
       </c>
-      <c r="R14" s="34">
+      <c r="R14" s="31">
         <v>0.108</v>
       </c>
-      <c r="S14" s="34">
+      <c r="S14" s="31">
         <f>R14*Q14</f>
         <v>2.7</v>
       </c>
-      <c r="T14" s="9">
+      <c r="T14" s="52">
         <f>ROW(T14) - ROW($A$1)</f>
         <v>13</v>
       </c>
@@ -2233,61 +2277,61 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="33" t="s">
         <v>82</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="35" t="s">
         <v>115</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>165</v>
+        <v>155</v>
+      </c>
+      <c r="J15" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L15" s="12">
-        <v>109541</v>
-      </c>
-      <c r="M15" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="N15" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O15" s="12">
+        <v>168</v>
+      </c>
+      <c r="L15" s="11">
+        <v>146588</v>
+      </c>
+      <c r="M15" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="N15" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O15" s="11">
         <v>1</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="47">
         <v>25</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="Q15" s="51">
         <f t="shared" ref="Q15" si="14">ROUNDUP(P15*N15,0)</f>
         <v>25</v>
       </c>
-      <c r="R15" s="34">
+      <c r="R15" s="31">
         <v>0.108</v>
       </c>
-      <c r="S15" s="34">
+      <c r="S15" s="31">
         <f t="shared" ref="S15" si="15">R15*Q15</f>
         <v>2.7</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="52">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
@@ -2297,61 +2341,61 @@
         <f>ROW(A16) - ROW($A$1)</f>
         <v>15</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="33" t="s">
         <v>83</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="35" t="s">
         <v>116</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>165</v>
+        <v>156</v>
+      </c>
+      <c r="J16" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L16" s="12">
-        <v>1844557</v>
-      </c>
-      <c r="M16" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="N16" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O16" s="12">
+        <v>168</v>
+      </c>
+      <c r="L16" s="11">
+        <v>1575659</v>
+      </c>
+      <c r="M16" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="N16" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O16" s="11">
         <v>8</v>
       </c>
-      <c r="P16" s="13">
+      <c r="P16" s="47">
         <v>200</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="Q16" s="51">
         <f>ROUNDUP(P16*N16,0)</f>
         <v>200</v>
       </c>
-      <c r="R16" s="34">
+      <c r="R16" s="31">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="S16" s="34">
+      <c r="S16" s="31">
         <f>R16*Q16</f>
         <v>1.6</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16" s="52">
         <f>ROW(T16) - ROW($A$1)</f>
         <v>15</v>
       </c>
@@ -2361,61 +2405,61 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="33" t="s">
         <v>83</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="35" t="s">
         <v>117</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>165</v>
+        <v>157</v>
+      </c>
+      <c r="J17" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L17" s="12">
-        <v>828858</v>
-      </c>
-      <c r="M17" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="N17" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O17" s="12">
+        <v>168</v>
+      </c>
+      <c r="L17" s="11">
+        <v>680225</v>
+      </c>
+      <c r="M17" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="N17" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O17" s="11">
         <v>2</v>
       </c>
-      <c r="P17" s="13">
+      <c r="P17" s="47">
         <v>50</v>
       </c>
-      <c r="Q17" s="13">
+      <c r="Q17" s="51">
         <f t="shared" ref="Q17" si="16">ROUNDUP(P17*N17,0)</f>
         <v>50</v>
       </c>
-      <c r="R17" s="34">
+      <c r="R17" s="31">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="S17" s="34">
+      <c r="S17" s="31">
         <f t="shared" ref="S17" si="17">R17*Q17</f>
         <v>0.65</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17" s="52">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -2425,61 +2469,61 @@
         <f>ROW(A18) - ROW($A$1)</f>
         <v>17</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="33" t="s">
         <v>83</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G18" s="38" t="s">
+      <c r="G18" s="35" t="s">
         <v>118</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>165</v>
+        <v>158</v>
+      </c>
+      <c r="J18" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L18" s="12">
-        <v>136009</v>
-      </c>
-      <c r="M18" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="N18" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O18" s="12">
+        <v>168</v>
+      </c>
+      <c r="L18" s="11">
+        <v>128297</v>
+      </c>
+      <c r="M18" s="50" t="s">
+        <v>187</v>
+      </c>
+      <c r="N18" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O18" s="11">
         <v>1</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="47">
         <v>25</v>
       </c>
-      <c r="Q18" s="13">
+      <c r="Q18" s="51">
         <f>ROUNDUP(P18*N18,0)</f>
         <v>25</v>
       </c>
-      <c r="R18" s="34">
+      <c r="R18" s="31">
         <v>0.04</v>
       </c>
-      <c r="S18" s="34">
+      <c r="S18" s="31">
         <f>R18*Q18</f>
         <v>1</v>
       </c>
-      <c r="T18" s="9">
+      <c r="T18" s="52">
         <f>ROW(T18) - ROW($A$1)</f>
         <v>17</v>
       </c>
@@ -2489,61 +2533,61 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="33" t="s">
         <v>83</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="35" t="s">
         <v>119</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>165</v>
+        <v>159</v>
+      </c>
+      <c r="J19" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L19" s="12">
-        <v>92176</v>
-      </c>
-      <c r="M19" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="N19" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O19" s="12">
+        <v>168</v>
+      </c>
+      <c r="L19" s="11">
+        <v>153762</v>
+      </c>
+      <c r="M19" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O19" s="11">
         <v>1</v>
       </c>
-      <c r="P19" s="13">
+      <c r="P19" s="47">
         <v>25</v>
       </c>
-      <c r="Q19" s="13">
+      <c r="Q19" s="51">
         <f t="shared" ref="Q19" si="18">ROUNDUP(P19*N19,0)</f>
         <v>25</v>
       </c>
-      <c r="R19" s="34">
-        <v>1.4E-2</v>
-      </c>
-      <c r="S19" s="34">
+      <c r="R19" s="31">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="S19" s="31">
         <f t="shared" ref="S19" si="19">R19*Q19</f>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="T19" s="9">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="T19" s="52">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -2553,61 +2597,61 @@
         <f>ROW(A20) - ROW($A$1)</f>
         <v>19</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="33" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="35" t="s">
         <v>120</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>165</v>
+        <v>160</v>
+      </c>
+      <c r="J20" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L20" s="12">
-        <v>1231971</v>
-      </c>
-      <c r="M20" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="N20" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O20" s="12">
+        <v>168</v>
+      </c>
+      <c r="L20" s="11">
+        <v>1039706</v>
+      </c>
+      <c r="M20" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O20" s="11">
         <v>2</v>
       </c>
-      <c r="P20" s="13">
+      <c r="P20" s="47">
         <v>50</v>
       </c>
-      <c r="Q20" s="13">
+      <c r="Q20" s="51">
         <f>ROUNDUP(P20*N20,0)</f>
         <v>50</v>
       </c>
-      <c r="R20" s="34">
+      <c r="R20" s="31">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="S20" s="34">
+      <c r="S20" s="31">
         <f>R20*Q20</f>
         <v>0.54999999999999993</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20" s="52">
         <f>ROW(T20) - ROW($A$1)</f>
         <v>19</v>
       </c>
@@ -2617,61 +2661,61 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="33" t="s">
         <v>84</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="35" t="s">
         <v>121</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>165</v>
+      <c r="J21" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L21" s="12">
-        <v>3171</v>
-      </c>
-      <c r="M21" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="N21" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O21" s="12">
+        <v>168</v>
+      </c>
+      <c r="L21" s="11">
+        <v>2855</v>
+      </c>
+      <c r="M21" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="N21" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O21" s="11">
         <v>3</v>
       </c>
-      <c r="P21" s="13">
+      <c r="P21" s="47">
         <v>75</v>
       </c>
-      <c r="Q21" s="13">
+      <c r="Q21" s="51">
         <f t="shared" ref="Q21" si="20">ROUNDUP(P21*N21,0)</f>
         <v>75</v>
       </c>
-      <c r="R21" s="34">
+      <c r="R21" s="31">
         <v>0.58899999999999997</v>
       </c>
-      <c r="S21" s="34">
+      <c r="S21" s="31">
         <f t="shared" ref="S21" si="21">R21*Q21</f>
         <v>44.174999999999997</v>
       </c>
-      <c r="T21" s="9">
+      <c r="T21" s="52">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -2681,61 +2725,61 @@
         <f>ROW(A22) - ROW($A$1)</f>
         <v>21</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="33" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="35" t="s">
         <v>122</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="J22" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L22" s="12">
-        <v>256</v>
-      </c>
-      <c r="M22" s="33" t="s">
-        <v>190</v>
-      </c>
-      <c r="N22" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O22" s="12">
+        <v>168</v>
+      </c>
+      <c r="L22" s="11">
+        <v>181</v>
+      </c>
+      <c r="M22" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="N22" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O22" s="11">
         <v>1</v>
       </c>
-      <c r="P22" s="13">
+      <c r="P22" s="47">
         <v>25</v>
       </c>
-      <c r="Q22" s="13">
+      <c r="Q22" s="51">
         <f>ROUNDUP(P22*N22,0)</f>
         <v>25</v>
       </c>
-      <c r="R22" s="34">
-        <v>3.83</v>
-      </c>
-      <c r="S22" s="34">
+      <c r="R22" s="31">
+        <v>3.76</v>
+      </c>
+      <c r="S22" s="31">
         <f>R22*Q22</f>
-        <v>95.75</v>
-      </c>
-      <c r="T22" s="9">
+        <v>94</v>
+      </c>
+      <c r="T22" s="52">
         <f>ROW(T22) - ROW($A$1)</f>
         <v>21</v>
       </c>
@@ -2745,61 +2789,61 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="33" t="s">
         <v>86</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="35" t="s">
         <v>123</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>165</v>
+        <v>162</v>
+      </c>
+      <c r="J23" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L23" s="12">
-        <v>12587</v>
-      </c>
-      <c r="M23" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="N23" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O23" s="12">
+        <v>168</v>
+      </c>
+      <c r="L23" s="11">
+        <v>11738</v>
+      </c>
+      <c r="M23" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="N23" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O23" s="11">
         <v>1</v>
       </c>
-      <c r="P23" s="13">
+      <c r="P23" s="47">
         <v>25</v>
       </c>
-      <c r="Q23" s="13">
+      <c r="Q23" s="51">
         <f t="shared" ref="Q23" si="22">ROUNDUP(P23*N23,0)</f>
         <v>25</v>
       </c>
-      <c r="R23" s="34">
+      <c r="R23" s="31">
         <v>0.63800000000000001</v>
       </c>
-      <c r="S23" s="34">
+      <c r="S23" s="31">
         <f t="shared" ref="S23" si="23">R23*Q23</f>
         <v>15.950000000000001</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23" s="52">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -2809,61 +2853,61 @@
         <f>ROW(A24) - ROW($A$1)</f>
         <v>23</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="33" t="s">
         <v>87</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="35" t="s">
         <v>124</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L24" s="12">
-        <v>3650</v>
-      </c>
-      <c r="M24" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="N24" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O24" s="12">
+        <v>168</v>
+      </c>
+      <c r="L24" s="11">
+        <v>4036</v>
+      </c>
+      <c r="M24" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="N24" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O24" s="11">
         <v>1</v>
       </c>
-      <c r="P24" s="13">
+      <c r="P24" s="47">
         <v>25</v>
       </c>
-      <c r="Q24" s="13">
+      <c r="Q24" s="51">
         <f>ROUNDUP(P24*N24,0)</f>
         <v>25</v>
       </c>
-      <c r="R24" s="34">
+      <c r="R24" s="31">
         <v>0.82299999999999995</v>
       </c>
-      <c r="S24" s="34">
+      <c r="S24" s="31">
         <f>R24*Q24</f>
         <v>20.574999999999999</v>
       </c>
-      <c r="T24" s="9">
+      <c r="T24" s="52">
         <f>ROW(T24) - ROW($A$1)</f>
         <v>23</v>
       </c>
@@ -2873,61 +2917,61 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="36" t="s">
+      <c r="C25" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="33" t="s">
         <v>88</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="38" t="s">
+      <c r="G25" s="35" t="s">
         <v>125</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="J25" s="49" t="s">
+        <v>166</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="L25" s="12">
-        <v>9046</v>
-      </c>
-      <c r="M25" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="N25" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O25" s="12">
+        <v>168</v>
+      </c>
+      <c r="L25" s="11">
+        <v>8964</v>
+      </c>
+      <c r="M25" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="N25" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O25" s="11">
         <v>1</v>
       </c>
-      <c r="P25" s="13">
+      <c r="P25" s="47">
         <v>25</v>
       </c>
-      <c r="Q25" s="13">
+      <c r="Q25" s="51">
         <f t="shared" ref="Q25" si="24">ROUNDUP(P25*N25,0)</f>
         <v>25</v>
       </c>
-      <c r="R25" s="34">
+      <c r="R25" s="31">
         <v>0.73099999999999998</v>
       </c>
-      <c r="S25" s="34">
+      <c r="S25" s="31">
         <f t="shared" ref="S25" si="25">R25*Q25</f>
         <v>18.274999999999999</v>
       </c>
-      <c r="T25" s="9">
+      <c r="T25" s="52">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
@@ -2937,20 +2981,20 @@
         <f>ROW(A26) - ROW($A$1)</f>
         <v>25</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="33" t="s">
         <v>68</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="35" t="s">
         <v>95</v>
       </c>
       <c r="H26" s="10" t="s">
@@ -2959,33 +3003,33 @@
       <c r="I26" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J26" s="11" t="s">
+      <c r="J26" s="49" t="s">
         <v>95</v>
       </c>
       <c r="K26" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="N26" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O26" s="12">
+      <c r="L26" s="11"/>
+      <c r="M26" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O26" s="11">
         <v>1</v>
       </c>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13">
+      <c r="P26" s="47"/>
+      <c r="Q26" s="51">
         <f>ROUNDUP(P26*N26,0)</f>
         <v>0</v>
       </c>
-      <c r="R26" s="34"/>
-      <c r="S26" s="34">
+      <c r="R26" s="31"/>
+      <c r="S26" s="31">
         <f>R26*Q26</f>
         <v>0</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="52">
         <f>ROW(T26) - ROW($A$1)</f>
         <v>25</v>
       </c>
@@ -2995,20 +3039,20 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G27" s="38" t="s">
+      <c r="G27" s="35" t="s">
         <v>95</v>
       </c>
       <c r="H27" s="10" t="s">
@@ -3017,33 +3061,33 @@
       <c r="I27" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="49" t="s">
         <v>95</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="N27" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O27" s="12">
+      <c r="L27" s="11"/>
+      <c r="M27" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="N27" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O27" s="11">
         <v>1</v>
       </c>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13">
+      <c r="P27" s="47"/>
+      <c r="Q27" s="51">
         <f t="shared" ref="Q27" si="26">ROUNDUP(P27*N27,0)</f>
         <v>0</v>
       </c>
-      <c r="R27" s="34"/>
-      <c r="S27" s="34">
+      <c r="R27" s="31"/>
+      <c r="S27" s="31">
         <f t="shared" ref="S27" si="27">R27*Q27</f>
         <v>0</v>
       </c>
-      <c r="T27" s="9">
+      <c r="T27" s="52">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -3053,20 +3097,20 @@
         <f>ROW(A28) - ROW($A$1)</f>
         <v>27</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="33" t="s">
         <v>90</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="35" t="s">
         <v>95</v>
       </c>
       <c r="H28" s="10" t="s">
@@ -3075,33 +3119,33 @@
       <c r="I28" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J28" s="11" t="s">
+      <c r="J28" s="49" t="s">
         <v>95</v>
       </c>
       <c r="K28" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L28" s="12"/>
-      <c r="M28" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="N28" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O28" s="12">
+      <c r="L28" s="11"/>
+      <c r="M28" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="N28" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O28" s="11">
         <v>1</v>
       </c>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13">
+      <c r="P28" s="47"/>
+      <c r="Q28" s="51">
         <f>ROUNDUP(P28*N28,0)</f>
         <v>0</v>
       </c>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34">
+      <c r="R28" s="31"/>
+      <c r="S28" s="31">
         <f>R28*Q28</f>
         <v>0</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28" s="52">
         <f>ROW(T28) - ROW($A$1)</f>
         <v>27</v>
       </c>
@@ -3111,20 +3155,20 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="33" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G29" s="38" t="s">
+      <c r="G29" s="35" t="s">
         <v>95</v>
       </c>
       <c r="H29" s="10" t="s">
@@ -3133,120 +3177,122 @@
       <c r="I29" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="49" t="s">
         <v>95</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="N29" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="O29" s="12">
+      <c r="L29" s="11"/>
+      <c r="M29" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="N29" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="O29" s="11">
         <v>1</v>
       </c>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13">
+      <c r="P29" s="47"/>
+      <c r="Q29" s="51">
         <f t="shared" ref="Q29" si="28">ROUNDUP(P29*N29,0)</f>
         <v>0</v>
       </c>
-      <c r="R29" s="34"/>
-      <c r="S29" s="34">
+      <c r="R29" s="31"/>
+      <c r="S29" s="31">
         <f t="shared" ref="S29" si="29">R29*Q29</f>
         <v>0</v>
       </c>
-      <c r="T29" s="9">
+      <c r="T29" s="52">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
     </row>
     <row r="31" spans="1:20" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="13"/>
+      <c r="C31" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="19"/>
-      <c r="F31" s="25" t="s">
+      <c r="E31" s="17"/>
+      <c r="F31" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G31" s="51" t="s">
+      <c r="G31" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="50" t="s">
+      <c r="H31" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="19"/>
-      <c r="K31" s="16" t="s">
+      <c r="I31" s="17"/>
+      <c r="K31" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="17"/>
-      <c r="M31" s="39">
+      <c r="L31" s="15"/>
+      <c r="M31" s="36">
         <f ca="1">NOW()</f>
-        <v>42296.623160648145</v>
-      </c>
-      <c r="N31" s="45"/>
-      <c r="O31" s="18"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="40" t="s">
+        <v>42314.460173495369</v>
+      </c>
+      <c r="N31" s="42"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="S31" s="41">
+      <c r="S31" s="38">
         <f>SUM(S2:S29)</f>
-        <v>376.28999999999991</v>
-      </c>
-      <c r="T31" s="49">
+        <v>372.41499999999991</v>
+      </c>
+      <c r="T31" s="46">
         <f>(SUM(T2:T29))/P32</f>
         <v>16.239999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M32" s="25" t="s">
+      <c r="M32" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="N32" s="46"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="52" t="s">
+      <c r="N32" s="43"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="43" t="s">
+      <c r="Q32" s="41"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="T32" s="48" t="s">
+      <c r="T32" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="16:16" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="P33" s="53"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>

</xml_diff>